<commit_message>
Update DR# 736 UCPB(Debit with Paywave) 05-25-2022.xlsx
</commit_message>
<xml_diff>
--- a/DR# 736 UCPB(Debit with Paywave) 05-25-2022.xlsx
+++ b/DR# 736 UCPB(Debit with Paywave) 05-25-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\GitHub\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9523B0-E03A-48F8-9B19-80AB961E35E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82346E2-2C4A-4E25-955C-6E7B6DFDCF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>DELIVERY RECEIPT</t>
   </si>
@@ -149,10 +149,16 @@
  Metro Manila</t>
   </si>
   <si>
-    <t>DR No. 000736</t>
-  </si>
-  <si>
-    <t>UCPB Debit w/ Paywave</t>
+    <t>DR No. 000352</t>
+  </si>
+  <si>
+    <t>PVC Cards (PANOLOKARDs)</t>
+  </si>
+  <si>
+    <t>Ribbons</t>
+  </si>
+  <si>
+    <t>Black Mono</t>
   </si>
 </sst>
 </file>
@@ -480,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -541,14 +547,14 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -556,6 +562,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -571,19 +592,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -970,7 +985,7 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1097,27 +1112,33 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="18.75">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="32" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="34">
-        <v>98000</v>
+        <v>150000</v>
       </c>
       <c r="D15" s="34">
-        <v>98000</v>
-      </c>
-      <c r="E15" s="31">
-        <v>44706</v>
-      </c>
+        <v>150000</v>
+      </c>
+      <c r="E15" s="31"/>
     </row>
     <row r="16" spans="1:13" ht="17.25" customHeight="1">
-      <c r="A16" s="25"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
+      <c r="A16" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="47">
+        <v>150</v>
+      </c>
+      <c r="D16" s="47">
+        <v>150</v>
+      </c>
       <c r="E16" s="26"/>
     </row>
     <row r="17" spans="1:5" ht="17.25" customHeight="1">
@@ -1154,12 +1175,12 @@
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="27">
-        <f>SUM(C15:C15)</f>
-        <v>98000</v>
+        <f>SUM(C15:C16)</f>
+        <v>150150</v>
       </c>
       <c r="D21" s="27">
-        <f>SUM(D15:D15)</f>
-        <v>98000</v>
+        <f>SUM(D15:D16)</f>
+        <v>150150</v>
       </c>
       <c r="E21" s="9"/>
     </row>
@@ -1198,7 +1219,7 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="89" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1335,10 +1356,10 @@
       <c r="B14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="46"/>
       <c r="E14" s="16" t="s">
         <v>12</v>
       </c>
@@ -1347,210 +1368,210 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="16.5">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="42" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="23">
         <v>1</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="43"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="22">
         <v>110000</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15" s="43">
         <v>44508</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="17.25" customHeight="1">
-      <c r="A16" s="37"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="23">
         <v>2</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="43"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="22">
         <v>150000</v>
       </c>
-      <c r="F16" s="38"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:6" ht="17.25" customHeight="1">
-      <c r="A17" s="37"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="23">
         <v>3</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="43"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="22">
         <v>102751</v>
       </c>
-      <c r="F17" s="38"/>
+      <c r="F17" s="43"/>
     </row>
     <row r="18" spans="1:6" ht="16.5">
-      <c r="A18" s="37"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="23">
         <v>4</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="43"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="22">
         <v>150000</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="43"/>
     </row>
     <row r="19" spans="1:6" ht="16.5">
-      <c r="A19" s="37"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="23">
         <v>5</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="43"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="22">
         <v>140000</v>
       </c>
-      <c r="F19" s="38"/>
+      <c r="F19" s="43"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
-      <c r="A20" s="37"/>
-      <c r="B20" s="39">
+      <c r="A20" s="42"/>
+      <c r="B20" s="44">
         <v>6</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="43"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="22">
         <v>47420</v>
       </c>
-      <c r="F20" s="38"/>
+      <c r="F20" s="43"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1">
-      <c r="A21" s="37"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="42" t="s">
+      <c r="A21" s="42"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="43"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="22">
         <v>14341</v>
       </c>
-      <c r="F21" s="38"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6" ht="16.5">
-      <c r="A22" s="37"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="23">
         <v>7</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="43"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="22">
         <v>150000</v>
       </c>
-      <c r="F22" s="38"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:6" ht="16.5">
-      <c r="A23" s="37"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="23">
         <v>8</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="43"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="22">
         <v>150000</v>
       </c>
-      <c r="F23" s="38"/>
+      <c r="F23" s="43"/>
     </row>
     <row r="24" spans="1:6" ht="16.5">
-      <c r="A24" s="37"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="23">
         <v>9</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="43"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="22">
         <v>150000</v>
       </c>
-      <c r="F24" s="38"/>
+      <c r="F24" s="43"/>
     </row>
     <row r="25" spans="1:6" ht="16.5">
-      <c r="A25" s="37"/>
+      <c r="A25" s="42"/>
       <c r="B25" s="23">
         <v>10</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="43"/>
+      <c r="D25" s="38"/>
       <c r="E25" s="22">
         <v>150000</v>
       </c>
-      <c r="F25" s="38"/>
+      <c r="F25" s="43"/>
     </row>
     <row r="26" spans="1:6" ht="16.5">
-      <c r="A26" s="37"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="23">
         <v>11</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="43"/>
+      <c r="D26" s="38"/>
       <c r="E26" s="22">
         <v>131366</v>
       </c>
-      <c r="F26" s="38"/>
+      <c r="F26" s="43"/>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1">
-      <c r="A27" s="37"/>
-      <c r="B27" s="39">
+      <c r="A27" s="42"/>
+      <c r="B27" s="44">
         <v>12</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="43"/>
+      <c r="D27" s="38"/>
       <c r="E27" s="22">
         <v>110037</v>
       </c>
-      <c r="F27" s="38"/>
+      <c r="F27" s="43"/>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
-      <c r="A28" s="37"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="42" t="s">
+      <c r="A28" s="42"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="43"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="22">
         <v>25756</v>
       </c>
-      <c r="F28" s="38"/>
+      <c r="F28" s="43"/>
     </row>
     <row r="29" spans="1:6" ht="16.5">
-      <c r="A29" s="37"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="23">
         <v>13</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="43"/>
+      <c r="D29" s="38"/>
       <c r="E29" s="22">
         <v>60000</v>
       </c>
@@ -1562,11 +1583,11 @@
       <c r="A30" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44" t="s">
+      <c r="B30" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="46"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="28">
         <f>SUM(E15:E29)</f>
         <v>1641671</v>
@@ -1591,13 +1612,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A15:A29"/>
@@ -1614,6 +1628,13 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>